<commit_message>
add ratio_scraper and store the stock list ratio into csv
</commit_message>
<xml_diff>
--- a/valuation/stock_data_2025-02-01.xlsx
+++ b/valuation/stock_data_2025-02-01.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yankesswang/Projects/PE_valuation/valuation/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413EA107-A774-A647-9154-EA7884919CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="大科技" sheetId="1" r:id="rId1"/>
@@ -20,7 +26,7 @@
     <sheet name="工業" sheetId="11" r:id="rId11"/>
     <sheet name="SaaS" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -2016,12 +2022,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2029,8 +2035,15 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -2069,24 +2082,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2124,7 +2148,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -2158,6 +2182,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2192,9 +2217,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2367,27 +2393,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
@@ -2655,7 +2681,7 @@
         <v>19</v>
       </c>
       <c r="B12">
-        <v>64.09999999999999</v>
+        <v>64.099999999999994</v>
       </c>
       <c r="C12">
         <v>43.9</v>
@@ -2673,7 +2699,7 @@
         <v>80.5</v>
       </c>
       <c r="H12">
-        <v>33.3</v>
+        <v>33.299999999999997</v>
       </c>
       <c r="I12">
         <v>26.2</v>
@@ -2763,7 +2789,7 @@
         <v>415.06</v>
       </c>
       <c r="I15">
-        <v>689.1799999999999</v>
+        <v>689.18</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -2915,34 +2941,35 @@
   <mergeCells count="1">
     <mergeCell ref="B1:I1"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>470</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
@@ -3089,7 +3116,7 @@
         <v>14</v>
       </c>
       <c r="B7">
-        <v>37.2</v>
+        <v>37.200000000000003</v>
       </c>
       <c r="C7">
         <v>64.12</v>
@@ -3110,7 +3137,7 @@
         <v>12.23</v>
       </c>
       <c r="I7">
-        <v>37.59</v>
+        <v>37.590000000000003</v>
       </c>
       <c r="J7">
         <v>39.86</v>
@@ -3127,7 +3154,7 @@
         <v>212.69</v>
       </c>
       <c r="C8">
-        <v>4.02</v>
+        <v>4.0199999999999996</v>
       </c>
       <c r="D8">
         <v>4.53</v>
@@ -3142,7 +3169,7 @@
         <v>2.79</v>
       </c>
       <c r="H8">
-        <v>5.06</v>
+        <v>5.0599999999999996</v>
       </c>
       <c r="I8">
         <v>14.37</v>
@@ -3151,7 +3178,7 @@
         <v>8.09</v>
       </c>
       <c r="K8">
-        <v>2.32</v>
+        <v>2.3199999999999998</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -3215,10 +3242,10 @@
         <v>5.56</v>
       </c>
       <c r="I10">
-        <v>17.35</v>
+        <v>17.350000000000001</v>
       </c>
       <c r="J10">
-        <v>9.390000000000001</v>
+        <v>9.39</v>
       </c>
       <c r="K10">
         <v>2.82</v>
@@ -3369,16 +3396,16 @@
         <v>22</v>
       </c>
       <c r="B15">
-        <v>4737.56</v>
+        <v>4737.5600000000004</v>
       </c>
       <c r="C15">
-        <v>158.23</v>
+        <v>158.22999999999999</v>
       </c>
       <c r="D15">
-        <v>131.17</v>
+        <v>131.16999999999999</v>
       </c>
       <c r="E15">
-        <v>290.59</v>
+        <v>290.58999999999997</v>
       </c>
       <c r="F15">
         <v>134.72</v>
@@ -3387,7 +3414,7 @@
         <v>45.83</v>
       </c>
       <c r="H15">
-        <v>86.84999999999999</v>
+        <v>86.85</v>
       </c>
       <c r="I15">
         <v>170.95</v>
@@ -3396,7 +3423,7 @@
         <v>256.07</v>
       </c>
       <c r="K15">
-        <v>34.48</v>
+        <v>34.479999999999997</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -3578,39 +3605,46 @@
   <mergeCells count="1">
     <mergeCell ref="B1:K1"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="1" width="30.59765625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.3984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>514</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="1" t="s">
@@ -3832,16 +3866,16 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>72.04000000000001</v>
+        <v>72.040000000000006</v>
       </c>
       <c r="H7">
-        <v>8.789999999999999</v>
+        <v>8.7899999999999991</v>
       </c>
       <c r="I7">
         <v>6.05</v>
       </c>
       <c r="J7">
-        <v>8.460000000000001</v>
+        <v>8.4600000000000009</v>
       </c>
       <c r="K7">
         <v>13.05</v>
@@ -3973,7 +4007,7 @@
         <v>14.26</v>
       </c>
       <c r="D10">
-        <v>4.56</v>
+        <v>4.5599999999999996</v>
       </c>
       <c r="E10">
         <v>8.69</v>
@@ -4079,19 +4113,19 @@
         <v>12.5</v>
       </c>
       <c r="F12">
-        <v>17.6</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="G12">
-        <v>90.40000000000001</v>
+        <v>90.4</v>
       </c>
       <c r="H12">
         <v>30</v>
       </c>
       <c r="I12">
-        <v>16.6</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="J12">
-        <v>16.4</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="K12">
         <v>31.4</v>
@@ -4226,7 +4260,7 @@
         <v>62.28</v>
       </c>
       <c r="E15">
-        <v>152.2</v>
+        <v>152.19999999999999</v>
       </c>
       <c r="F15">
         <v>52.31</v>
@@ -4516,40 +4550,41 @@
   <mergeCells count="1">
     <mergeCell ref="B1:P1"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:Q20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>587</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="1" t="s">
@@ -4780,7 +4815,7 @@
         <v>38.07</v>
       </c>
       <c r="F7">
-        <v>157.98</v>
+        <v>157.97999999999999</v>
       </c>
       <c r="G7">
         <v>42.8</v>
@@ -4801,13 +4836,13 @@
         <v>0</v>
       </c>
       <c r="M7">
-        <v>39.12</v>
+        <v>39.119999999999997</v>
       </c>
       <c r="N7">
         <v>0</v>
       </c>
       <c r="O7">
-        <v>40.2</v>
+        <v>40.200000000000003</v>
       </c>
       <c r="P7">
         <v>0</v>
@@ -4824,7 +4859,7 @@
         <v>6.21</v>
       </c>
       <c r="C8">
-        <v>10.13</v>
+        <v>10.130000000000001</v>
       </c>
       <c r="D8">
         <v>12.94</v>
@@ -4836,7 +4871,7 @@
         <v>1.55</v>
       </c>
       <c r="G8">
-        <v>19.67</v>
+        <v>19.670000000000002</v>
       </c>
       <c r="H8">
         <v>2.82</v>
@@ -4845,7 +4880,7 @@
         <v>7.3</v>
       </c>
       <c r="J8">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="K8">
         <v>1.95</v>
@@ -4948,7 +4983,7 @@
         <v>3</v>
       </c>
       <c r="I10">
-        <v>8.550000000000001</v>
+        <v>8.5500000000000007</v>
       </c>
       <c r="J10">
         <v>5.62</v>
@@ -4972,7 +5007,7 @@
         <v>0.51</v>
       </c>
       <c r="Q10">
-        <v>2.53</v>
+        <v>2.5299999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -5201,7 +5236,7 @@
         <v>384.95</v>
       </c>
       <c r="E15">
-        <v>311.34</v>
+        <v>311.33999999999997</v>
       </c>
       <c r="F15">
         <v>116.8</v>
@@ -5216,7 +5251,7 @@
         <v>262.06</v>
       </c>
       <c r="J15">
-        <v>86.95999999999999</v>
+        <v>86.96</v>
       </c>
       <c r="K15">
         <v>118.68</v>
@@ -5509,32 +5544,33 @@
   <mergeCells count="1">
     <mergeCell ref="B1:Q1"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
@@ -5663,7 +5699,7 @@
         <v>7.68</v>
       </c>
       <c r="D7">
-        <v>20.4</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="E7">
         <v>114.48</v>
@@ -5744,7 +5780,7 @@
         <v>17</v>
       </c>
       <c r="B10">
-        <v>8.369999999999999</v>
+        <v>8.3699999999999992</v>
       </c>
       <c r="C10">
         <v>14.46</v>
@@ -5904,13 +5940,13 @@
         <v>176.52</v>
       </c>
       <c r="G15">
-        <v>266.6</v>
+        <v>266.60000000000002</v>
       </c>
       <c r="H15">
         <v>73.25</v>
       </c>
       <c r="I15">
-        <v>16.92</v>
+        <v>16.920000000000002</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -6062,31 +6098,32 @@
   <mergeCells count="1">
     <mergeCell ref="B1:I1"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
@@ -6232,13 +6269,13 @@
         <v>5.6</v>
       </c>
       <c r="E8">
-        <v>17.06</v>
+        <v>17.059999999999999</v>
       </c>
       <c r="F8">
         <v>7.39</v>
       </c>
       <c r="G8">
-        <v>0.29</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="H8">
         <v>43.91</v>
@@ -6287,7 +6324,7 @@
         <v>18.48</v>
       </c>
       <c r="F10">
-        <v>9.210000000000001</v>
+        <v>9.2100000000000009</v>
       </c>
       <c r="G10">
         <v>0.49</v>
@@ -6417,7 +6454,7 @@
         <v>267.3</v>
       </c>
       <c r="F15">
-        <v>81.43000000000001</v>
+        <v>81.430000000000007</v>
       </c>
       <c r="G15">
         <v>15.78</v>
@@ -6560,30 +6597,31 @@
   <mergeCells count="1">
     <mergeCell ref="B1:H1"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
@@ -6688,7 +6726,7 @@
         <v>39.33</v>
       </c>
       <c r="D7">
-        <v>33.41</v>
+        <v>33.409999999999997</v>
       </c>
       <c r="E7">
         <v>74</v>
@@ -6697,7 +6735,7 @@
         <v>1.44</v>
       </c>
       <c r="G7">
-        <v>8.640000000000001</v>
+        <v>8.64</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -7003,28 +7041,29 @@
   <mergeCells count="1">
     <mergeCell ref="B1:G1"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
@@ -7116,7 +7155,7 @@
         <v>15</v>
       </c>
       <c r="B8">
-        <v>4.98</v>
+        <v>4.9800000000000004</v>
       </c>
       <c r="C8">
         <v>16.79</v>
@@ -7184,7 +7223,7 @@
         <v>19</v>
       </c>
       <c r="B12">
-        <v>39.2</v>
+        <v>39.200000000000003</v>
       </c>
       <c r="C12">
         <v>36.6</v>
@@ -7238,7 +7277,7 @@
         <v>88.58</v>
       </c>
       <c r="C15">
-        <v>555.4299999999999</v>
+        <v>555.42999999999995</v>
       </c>
       <c r="D15">
         <v>341.8</v>
@@ -7336,35 +7375,36 @@
   <mergeCells count="1">
     <mergeCell ref="B1:E1"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
@@ -7553,7 +7593,7 @@
         <v>64.86</v>
       </c>
       <c r="L7">
-        <v>8.199999999999999</v>
+        <v>8.1999999999999993</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -7567,7 +7607,7 @@
         <v>4.58</v>
       </c>
       <c r="D8">
-        <v>18.58</v>
+        <v>18.579999999999998</v>
       </c>
       <c r="E8">
         <v>11.83</v>
@@ -7640,10 +7680,10 @@
         <v>6.11</v>
       </c>
       <c r="C10">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="D10">
-        <v>20.35</v>
+        <v>20.350000000000001</v>
       </c>
       <c r="E10">
         <v>12.47</v>
@@ -7740,7 +7780,7 @@
         <v>11.1</v>
       </c>
       <c r="K12">
-        <v>10.2</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="L12">
         <v>24</v>
@@ -7836,16 +7876,16 @@
         <v>979.88</v>
       </c>
       <c r="E15">
-        <v>89.59999999999999</v>
+        <v>89.6</v>
       </c>
       <c r="F15">
-        <v>76.90000000000001</v>
+        <v>76.900000000000006</v>
       </c>
       <c r="G15">
         <v>414.2</v>
       </c>
       <c r="H15">
-        <v>83.43000000000001</v>
+        <v>83.43</v>
       </c>
       <c r="I15">
         <v>20.05</v>
@@ -8054,42 +8094,43 @@
   <mergeCells count="1">
     <mergeCell ref="B1:L1"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="1" t="s">
@@ -8344,7 +8385,7 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>9.130000000000001</v>
+        <v>9.1300000000000008</v>
       </c>
       <c r="G7">
         <v>65.02</v>
@@ -8374,7 +8415,7 @@
         <v>0</v>
       </c>
       <c r="P7">
-        <v>32.27</v>
+        <v>32.270000000000003</v>
       </c>
       <c r="Q7">
         <v>-7.56</v>
@@ -8403,7 +8444,7 @@
         <v>0.6</v>
       </c>
       <c r="F8">
-        <v>8.699999999999999</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="G8">
         <v>3.55</v>
@@ -8412,7 +8453,7 @@
         <v>3.18</v>
       </c>
       <c r="I8">
-        <v>0.55</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J8">
         <v>17.7</v>
@@ -8524,7 +8565,7 @@
         <v>9.35</v>
       </c>
       <c r="G10">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="H10">
         <v>3.79</v>
@@ -8533,7 +8574,7 @@
         <v>0.73</v>
       </c>
       <c r="J10">
-        <v>19.58</v>
+        <v>19.579999999999998</v>
       </c>
       <c r="K10">
         <v>13.79</v>
@@ -8551,7 +8592,7 @@
         <v>2.15</v>
       </c>
       <c r="P10">
-        <v>4.14</v>
+        <v>4.1399999999999997</v>
       </c>
       <c r="Q10">
         <v>2.1</v>
@@ -8627,10 +8668,10 @@
         <v>19</v>
       </c>
       <c r="B12">
-        <v>91.09999999999999</v>
+        <v>91.1</v>
       </c>
       <c r="C12">
-        <v>34.3</v>
+        <v>34.299999999999997</v>
       </c>
       <c r="D12">
         <v>24.3</v>
@@ -8672,7 +8713,7 @@
         <v>16.2</v>
       </c>
       <c r="Q12">
-        <v>9.699999999999999</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="R12">
         <v>13.9</v>
@@ -9157,40 +9198,60 @@
   <mergeCells count="1">
     <mergeCell ref="B1:S1"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="1" width="30.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="8.796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.3984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="8.796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.3984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="1" t="s">
@@ -9415,7 +9476,7 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>147.36</v>
+        <v>147.36000000000001</v>
       </c>
       <c r="E7">
         <v>100.84</v>
@@ -9433,7 +9494,7 @@
         <v>67.38</v>
       </c>
       <c r="J7">
-        <v>66.81999999999999</v>
+        <v>66.819999999999993</v>
       </c>
       <c r="K7">
         <v>171.54</v>
@@ -9483,16 +9544,16 @@
         <v>7.98</v>
       </c>
       <c r="I8">
-        <v>4.48</v>
+        <v>4.4800000000000004</v>
       </c>
       <c r="J8">
         <v>3.01</v>
       </c>
       <c r="K8">
-        <v>5.11</v>
+        <v>5.1100000000000003</v>
       </c>
       <c r="L8">
-        <v>4.85</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="M8">
         <v>5.51</v>
@@ -9607,7 +9668,7 @@
         <v>29.32</v>
       </c>
       <c r="O10">
-        <v>2.28</v>
+        <v>2.2799999999999998</v>
       </c>
       <c r="P10">
         <v>12.39</v>
@@ -9686,7 +9747,7 @@
         <v>8.6</v>
       </c>
       <c r="F12">
-        <v>265.9</v>
+        <v>265.89999999999998</v>
       </c>
       <c r="G12">
         <v>22.8</v>
@@ -9716,7 +9777,7 @@
         <v>10.3</v>
       </c>
       <c r="P12">
-        <v>16.6</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="Q12">
         <v>33</v>
@@ -9839,13 +9900,13 @@
         <v>112.86</v>
       </c>
       <c r="D15">
-        <v>91.23999999999999</v>
+        <v>91.24</v>
       </c>
       <c r="E15">
         <v>19.43</v>
       </c>
       <c r="F15">
-        <v>159.55</v>
+        <v>159.55000000000001</v>
       </c>
       <c r="G15">
         <v>209.32</v>
@@ -9866,10 +9927,10 @@
         <v>82.98</v>
       </c>
       <c r="M15">
-        <v>88.76000000000001</v>
+        <v>88.76</v>
       </c>
       <c r="N15">
-        <v>739.3099999999999</v>
+        <v>739.31</v>
       </c>
       <c r="O15">
         <v>21.19</v>
@@ -10150,29 +10211,30 @@
   <mergeCells count="1">
     <mergeCell ref="B1:Q1"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>449</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
@@ -10279,7 +10341,7 @@
         <v>15</v>
       </c>
       <c r="B8">
-        <v>8.130000000000001</v>
+        <v>8.1300000000000008</v>
       </c>
       <c r="C8">
         <v>3.49</v>
@@ -10291,7 +10353,7 @@
         <v>7.85</v>
       </c>
       <c r="F8">
-        <v>8.199999999999999</v>
+        <v>8.1999999999999993</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -10331,7 +10393,7 @@
         <v>9.23</v>
       </c>
       <c r="F10">
-        <v>9.359999999999999</v>
+        <v>9.36</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -10368,7 +10430,7 @@
         <v>10.6</v>
       </c>
       <c r="E12">
-        <v>10.2</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="F12">
         <v>9.6</v>
@@ -10538,6 +10600,7 @@
   <mergeCells count="1">
     <mergeCell ref="B1:F1"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>